<commit_message>
Added Software License Assignments
Added software license tracking
</commit_message>
<xml_diff>
--- a/IT_Inventory-Template.xlsx
+++ b/IT_Inventory-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1e0d50971877758/Documents/Working/IIDP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1e0d50971877758/Documents/IID/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACB6C1F8-2300-4FE9-AFA0-AB917008DC8A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{ACB6C1F8-2300-4FE9-AFA0-AB917008DC8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99ADF9E4-F3AA-4C1B-8334-A12D9403477B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="Network Equipment" sheetId="5" r:id="rId5"/>
     <sheet name="Other Equipment" sheetId="6" r:id="rId6"/>
     <sheet name="Account Information" sheetId="7" r:id="rId7"/>
+    <sheet name="Software Licenses" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>Hostname</t>
   </si>
@@ -128,6 +129,24 @@
   </si>
   <si>
     <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>License Key</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Assigned Date</t>
   </si>
 </sst>
 </file>
@@ -793,6 +812,21 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Phone Number" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{05F458B4-D727-40CF-AFDB-6D64AA125708}" name="Table8" displayName="Table8" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{04794439-DD6B-4D51-B185-F9182FCED1FE}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2ADDE3FE-969B-4BF9-AC93-223868816A34}" name="Company"/>
+    <tableColumn id="2" xr3:uid="{EB290B3A-6333-45E5-A5A5-63CE15897758}" name="Software"/>
+    <tableColumn id="3" xr3:uid="{08031ED1-87F3-4C6F-A9AE-A89392EE3FDC}" name="Version"/>
+    <tableColumn id="4" xr3:uid="{3F7016BC-7A54-4C06-8262-E28683CEC6DC}" name="License Key"/>
+    <tableColumn id="5" xr3:uid="{6AF91515-4853-4EEB-BEED-34D5E4E1A77E}" name="Assigned To"/>
+    <tableColumn id="6" xr3:uid="{CB35BA3E-8651-47A7-858D-D44A006A3453}" name="Assigned Date"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1119,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -1580,4 +1614,50 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96336563-E923-4BF3-8673-3DDFB84D0244}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="10.09765625" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="12.09765625" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>